<commit_message>
actualizo a 9 oct 4 pm
</commit_message>
<xml_diff>
--- a/competencia 01 bitácora.xlsx
+++ b/competencia 01 bitácora.xlsx
@@ -16,13 +16,13 @@
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="H10">
+    <comment authorId="0" ref="H13">
       <text>
         <t xml:space="preserve">pocos hiperparametros
 	-Silvana Contreras</t>
       </text>
     </comment>
-    <comment authorId="0" ref="C8">
+    <comment authorId="0" ref="C11">
       <text>
         <t xml:space="preserve">lags y deltas 1, aguinaldo, mpayroll normalizado
 	-Silvana Contreras</t>
@@ -34,7 +34,7 @@
 	-Silvana Contreras</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I8">
+    <comment authorId="0" ref="I11">
       <text>
         <t xml:space="preserve">fe2= aguinaldos, saldos normalizados
 	-Silvana Contreras</t>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="57">
   <si>
     <t>dataset</t>
   </si>
@@ -124,7 +124,7 @@
     <t>1,2,3</t>
   </si>
   <si>
-    <t>stop #30 0.9441</t>
+    <t>auc 0.9441</t>
   </si>
   <si>
     <t>6 seeds</t>
@@ -133,25 +133,31 @@
     <t>10500-12000, 13500</t>
   </si>
   <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>fe lags deltas 1,2,3 (9005)</t>
+  </si>
+  <si>
     <t>9002 auc 0.9441</t>
+  </si>
+  <si>
+    <t>1,2,3,4</t>
+  </si>
+  <si>
+    <t>10 seeds</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>1000, 12000, 13500</t>
   </si>
   <si>
     <t>fe lags deltas 1</t>
   </si>
   <si>
-    <t>10 seeds</t>
-  </si>
-  <si>
-    <t>*</t>
-  </si>
-  <si>
-    <t>1,2,3,4</t>
-  </si>
-  <si>
     <t>7 seeds</t>
-  </si>
-  <si>
-    <t>null</t>
   </si>
   <si>
     <t>fe1yag ídem fe1</t>
@@ -181,7 +187,7 @@
     <t xml:space="preserve">optimizar fe1 </t>
   </si>
   <si>
-    <t>COLAB</t>
+    <t>auc 0.9457</t>
   </si>
   <si>
     <t xml:space="preserve">fe lags deltas 1,2,3 </t>
@@ -190,19 +196,19 @@
     <t xml:space="preserve">fe lags deltas 1,2,3 y ag </t>
   </si>
   <si>
+    <t>fe123_rank</t>
+  </si>
+  <si>
+    <t>auc = 0.9447</t>
+  </si>
+  <si>
+    <t>fe123_rank_agui</t>
+  </si>
+  <si>
     <t>rserver</t>
   </si>
   <si>
-    <t>RANKINGS</t>
-  </si>
-  <si>
-    <t>fe lags deltas 1,2,3 (9005)</t>
-  </si>
-  <si>
-    <t>1000, 12000, 13500</t>
-  </si>
-  <si>
-    <t>local</t>
+    <t>9002 new 0.9448/50</t>
   </si>
   <si>
     <t>yo pienso que 9013 es el mejor aunque no es el mejor en kaggle</t>
@@ -213,12 +219,15 @@
   <si>
     <t>terminar de optimizar 9002 con min data 3</t>
   </si>
+  <si>
+    <t>colab</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="20">
+  <fonts count="22">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -270,6 +279,17 @@
     </font>
     <font>
       <b/>
+      <color rgb="FF4285F4"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="8.0"/>
       <color theme="4"/>
       <name val="Arial"/>
@@ -283,6 +303,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <color rgb="FF38761D"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -301,21 +328,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8.0"/>
-      <color rgb="FF000000"/>
+      <b/>
+      <color rgb="FF85200C"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11.0"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <color rgb="FF4285F4"/>
+      <sz val="8.0"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -333,13 +353,14 @@
     </font>
     <font>
       <b/>
-      <color rgb="FF38761D"/>
+      <sz val="11.0"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <color rgb="FFFF0000"/>
+      <sz val="9.0"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -389,8 +410,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFE6B8AF"/>
+        <bgColor rgb="FFE6B8AF"/>
       </patternFill>
     </fill>
   </fills>
@@ -400,7 +421,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="77">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -453,97 +474,119 @@
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="5" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="5" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="15" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="6" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="6" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="6" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="12" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="6" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="6" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="6" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="6" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="6" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="6" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="6" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="19" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="7" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="7" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="7" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="7" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="7" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="7" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="7" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="7" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="7" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="4" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="8" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="4" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
@@ -556,43 +599,29 @@
     <xf borderId="0" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="8" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="8" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="8" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="8" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="8" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="8" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="8" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="10" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="5" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="8" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
@@ -1059,13 +1088,13 @@
       <c r="E5" s="16">
         <v>0.2</v>
       </c>
-      <c r="F5" s="16">
-        <v>80.0</v>
+      <c r="F5" s="17">
+        <v>30.0</v>
       </c>
       <c r="G5" s="16">
         <v>11.0</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="H5" s="17" t="s">
         <v>24</v>
       </c>
       <c r="I5" s="15" t="s">
@@ -1074,7 +1103,7 @@
       <c r="J5" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="K5" s="16" t="s">
+      <c r="K5" s="18" t="s">
         <v>25</v>
       </c>
       <c r="L5" s="16">
@@ -1089,739 +1118,817 @@
       <c r="O5" s="16">
         <v>8.0</v>
       </c>
-      <c r="P5" s="17" t="s">
+      <c r="P5" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="Q5" s="18"/>
-      <c r="R5" s="18"/>
-      <c r="S5" s="18"/>
-      <c r="T5" s="18"/>
-      <c r="U5" s="18"/>
-      <c r="V5" s="18"/>
-      <c r="W5" s="18"/>
-      <c r="X5" s="18"/>
-      <c r="Y5" s="18"/>
-      <c r="Z5" s="18"/>
-      <c r="AA5" s="18"/>
-      <c r="AB5" s="18"/>
-      <c r="AC5" s="18"/>
-      <c r="AD5" s="18"/>
-      <c r="AE5" s="18"/>
-      <c r="AF5" s="18"/>
-      <c r="AG5" s="18"/>
-      <c r="AH5" s="18"/>
-      <c r="AI5" s="18"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="20"/>
+      <c r="S5" s="20"/>
+      <c r="T5" s="20"/>
+      <c r="U5" s="20"/>
+      <c r="V5" s="20"/>
+      <c r="W5" s="20"/>
+      <c r="X5" s="20"/>
+      <c r="Y5" s="20"/>
+      <c r="Z5" s="20"/>
+      <c r="AA5" s="20"/>
+      <c r="AB5" s="20"/>
+      <c r="AC5" s="20"/>
+      <c r="AD5" s="20"/>
+      <c r="AE5" s="20"/>
+      <c r="AF5" s="20"/>
+      <c r="AG5" s="20"/>
+      <c r="AH5" s="20"/>
+      <c r="AI5" s="20"/>
     </row>
     <row r="6">
-      <c r="A6" s="19"/>
-      <c r="B6" s="19">
+      <c r="A6" s="21"/>
+      <c r="B6" s="14">
+        <v>9002.0</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="16">
+        <v>0.2</v>
+      </c>
+      <c r="F6" s="16">
+        <v>80.0</v>
+      </c>
+      <c r="G6" s="16">
+        <v>11.0</v>
+      </c>
+      <c r="H6" s="17"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="24"/>
+      <c r="Q6" s="25"/>
+      <c r="R6" s="25"/>
+      <c r="S6" s="25"/>
+      <c r="T6" s="25"/>
+      <c r="U6" s="25"/>
+      <c r="V6" s="25"/>
+      <c r="W6" s="25"/>
+      <c r="X6" s="25"/>
+      <c r="Y6" s="25"/>
+      <c r="Z6" s="25"/>
+      <c r="AA6" s="25"/>
+      <c r="AB6" s="25"/>
+      <c r="AC6" s="25"/>
+      <c r="AD6" s="25"/>
+      <c r="AE6" s="25"/>
+      <c r="AF6" s="25"/>
+      <c r="AG6" s="25"/>
+      <c r="AH6" s="25"/>
+      <c r="AI6" s="25"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="21">
+        <v>9013.0</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="18">
+        <v>0.2</v>
+      </c>
+      <c r="F7" s="26"/>
+      <c r="G7" s="18">
+        <v>11.0</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="K7" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="L7" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="M7" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="N7" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="O7" s="23">
+        <v>7.0</v>
+      </c>
+      <c r="P7" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q7" s="25"/>
+      <c r="R7" s="25"/>
+      <c r="S7" s="25"/>
+      <c r="T7" s="25"/>
+      <c r="U7" s="25"/>
+      <c r="V7" s="25"/>
+      <c r="W7" s="25"/>
+      <c r="X7" s="25"/>
+      <c r="Y7" s="25"/>
+      <c r="Z7" s="25"/>
+      <c r="AA7" s="25"/>
+      <c r="AB7" s="25"/>
+      <c r="AC7" s="25"/>
+      <c r="AD7" s="25"/>
+      <c r="AE7" s="25"/>
+      <c r="AF7" s="25"/>
+      <c r="AG7" s="25"/>
+      <c r="AH7" s="25"/>
+      <c r="AI7" s="25"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="27"/>
+      <c r="B8" s="27">
         <v>9004.0</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C8" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D8" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E8" s="29">
         <v>0.2</v>
       </c>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21">
+      <c r="F8" s="29"/>
+      <c r="G8" s="29">
         <v>11.0</v>
       </c>
-      <c r="H6" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="J6" s="23">
+      <c r="H8" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="J8" s="31">
         <v>2.0</v>
       </c>
-      <c r="K6" s="23" t="s">
+      <c r="K8" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="L8" s="31">
+        <v>3.0</v>
+      </c>
+      <c r="M8" s="31">
+        <v>10000.0</v>
+      </c>
+      <c r="N8" s="31">
+        <v>2.544E8</v>
+      </c>
+      <c r="O8" s="29">
+        <v>7.0</v>
+      </c>
+      <c r="P8" s="32"/>
+      <c r="Q8" s="32"/>
+      <c r="R8" s="32"/>
+      <c r="S8" s="32"/>
+      <c r="T8" s="32"/>
+      <c r="U8" s="32"/>
+      <c r="V8" s="32"/>
+      <c r="W8" s="32"/>
+      <c r="X8" s="32"/>
+      <c r="Y8" s="32"/>
+      <c r="Z8" s="32"/>
+      <c r="AA8" s="32"/>
+      <c r="AB8" s="32"/>
+      <c r="AC8" s="32"/>
+      <c r="AD8" s="32"/>
+      <c r="AE8" s="32"/>
+      <c r="AF8" s="32"/>
+      <c r="AG8" s="32"/>
+      <c r="AH8" s="32"/>
+      <c r="AI8" s="32"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="33"/>
+      <c r="B9" s="34">
+        <v>9014.0</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="36">
+        <v>0.2</v>
+      </c>
+      <c r="F9" s="37"/>
+      <c r="G9" s="36">
+        <v>11.0</v>
+      </c>
+      <c r="H9" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="L6" s="23">
-        <v>3.0</v>
-      </c>
-      <c r="M6" s="23">
+      <c r="I9" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="J9" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="K9" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="L9" s="36">
+        <v>4.0</v>
+      </c>
+      <c r="M9" s="36">
+        <v>9000.0</v>
+      </c>
+      <c r="N9" s="36">
+        <v>3.544E8</v>
+      </c>
+      <c r="O9" s="37"/>
+      <c r="P9" s="38"/>
+      <c r="Q9" s="38"/>
+      <c r="R9" s="38"/>
+      <c r="S9" s="38"/>
+      <c r="T9" s="38"/>
+      <c r="U9" s="38"/>
+      <c r="V9" s="38"/>
+      <c r="W9" s="38"/>
+      <c r="X9" s="38"/>
+      <c r="Y9" s="38"/>
+      <c r="Z9" s="38"/>
+      <c r="AA9" s="38"/>
+      <c r="AB9" s="38"/>
+      <c r="AC9" s="38"/>
+      <c r="AD9" s="38"/>
+      <c r="AE9" s="38"/>
+      <c r="AF9" s="38"/>
+      <c r="AG9" s="38"/>
+      <c r="AH9" s="38"/>
+      <c r="AI9" s="38"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="33"/>
+      <c r="B10" s="33">
+        <v>9005.0</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="36">
+        <v>0.2</v>
+      </c>
+      <c r="F10" s="37"/>
+      <c r="G10" s="36">
+        <v>11.0</v>
+      </c>
+      <c r="H10" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="I10" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="J10" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="K10" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="L10" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="M10" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="N10" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="O10" s="36">
+        <v>8.0</v>
+      </c>
+      <c r="P10" s="36">
+        <v>13500.0</v>
+      </c>
+      <c r="Q10" s="38"/>
+      <c r="R10" s="38"/>
+      <c r="S10" s="38"/>
+      <c r="T10" s="38"/>
+      <c r="U10" s="38"/>
+      <c r="V10" s="38"/>
+      <c r="W10" s="38"/>
+      <c r="X10" s="38"/>
+      <c r="Y10" s="38"/>
+      <c r="Z10" s="38"/>
+      <c r="AA10" s="38"/>
+      <c r="AB10" s="38"/>
+      <c r="AC10" s="38"/>
+      <c r="AD10" s="38"/>
+      <c r="AE10" s="38"/>
+      <c r="AF10" s="38"/>
+      <c r="AG10" s="38"/>
+      <c r="AH10" s="38"/>
+      <c r="AI10" s="38"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="39"/>
+      <c r="B11" s="39">
+        <v>9006.0</v>
+      </c>
+      <c r="C11" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="41">
+        <v>0.2</v>
+      </c>
+      <c r="F11" s="41">
+        <v>35.0</v>
+      </c>
+      <c r="G11" s="41">
+        <v>5.0</v>
+      </c>
+      <c r="H11" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="J11" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="K11" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="L11" s="41">
+        <v>4.0</v>
+      </c>
+      <c r="M11" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="N11" s="41">
+        <v>3.408E8</v>
+      </c>
+      <c r="O11" s="41">
+        <v>6.0</v>
+      </c>
+      <c r="P11" s="44"/>
+      <c r="Q11" s="44"/>
+      <c r="R11" s="44"/>
+      <c r="S11" s="44"/>
+      <c r="T11" s="44"/>
+      <c r="U11" s="44"/>
+      <c r="V11" s="44"/>
+      <c r="W11" s="44"/>
+      <c r="X11" s="44"/>
+      <c r="Y11" s="44"/>
+      <c r="Z11" s="44"/>
+      <c r="AA11" s="44"/>
+      <c r="AB11" s="44"/>
+      <c r="AC11" s="44"/>
+      <c r="AD11" s="44"/>
+      <c r="AE11" s="44"/>
+      <c r="AF11" s="44"/>
+      <c r="AG11" s="44"/>
+      <c r="AH11" s="44"/>
+      <c r="AI11" s="44"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="45"/>
+      <c r="B12" s="45">
+        <v>9007.0</v>
+      </c>
+      <c r="C12" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="47">
+        <v>0.2</v>
+      </c>
+      <c r="F12" s="47">
+        <v>35.0</v>
+      </c>
+      <c r="G12" s="47">
+        <v>5.0</v>
+      </c>
+      <c r="H12" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="I12" s="46" t="s">
+        <v>38</v>
+      </c>
+      <c r="J12" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="K12" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="L12" s="47"/>
+      <c r="M12" s="47"/>
+      <c r="N12" s="47"/>
+      <c r="O12" s="48"/>
+      <c r="P12" s="49"/>
+      <c r="Q12" s="49"/>
+      <c r="R12" s="49"/>
+      <c r="S12" s="49"/>
+      <c r="T12" s="49"/>
+      <c r="U12" s="49"/>
+      <c r="V12" s="49"/>
+      <c r="W12" s="49"/>
+      <c r="X12" s="49"/>
+      <c r="Y12" s="49"/>
+      <c r="Z12" s="49"/>
+      <c r="AA12" s="49"/>
+      <c r="AB12" s="49"/>
+      <c r="AC12" s="49"/>
+      <c r="AD12" s="49"/>
+      <c r="AE12" s="49"/>
+      <c r="AF12" s="49"/>
+      <c r="AG12" s="49"/>
+      <c r="AH12" s="49"/>
+      <c r="AI12" s="49"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="50"/>
+      <c r="B13" s="50">
+        <v>9008.0</v>
+      </c>
+      <c r="C13" s="51" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="52">
+        <v>0.2</v>
+      </c>
+      <c r="F13" s="52">
+        <v>35.0</v>
+      </c>
+      <c r="G13" s="52">
+        <v>5.0</v>
+      </c>
+      <c r="H13" s="51" t="s">
+        <v>40</v>
+      </c>
+      <c r="I13" s="53" t="s">
+        <v>42</v>
+      </c>
+      <c r="J13" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="K13" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="L13" s="52">
+        <v>4.0</v>
+      </c>
+      <c r="M13" s="52">
+        <v>11000.0</v>
+      </c>
+      <c r="N13" s="52">
+        <v>3.392E8</v>
+      </c>
+      <c r="O13" s="52">
+        <v>7.0</v>
+      </c>
+      <c r="P13" s="54"/>
+      <c r="Q13" s="54"/>
+      <c r="R13" s="54"/>
+      <c r="S13" s="54"/>
+      <c r="T13" s="54"/>
+      <c r="U13" s="54"/>
+      <c r="V13" s="54"/>
+      <c r="W13" s="54"/>
+      <c r="X13" s="54"/>
+      <c r="Y13" s="54"/>
+      <c r="Z13" s="54"/>
+      <c r="AA13" s="54"/>
+      <c r="AB13" s="54"/>
+      <c r="AC13" s="54"/>
+      <c r="AD13" s="54"/>
+      <c r="AE13" s="54"/>
+      <c r="AF13" s="54"/>
+      <c r="AG13" s="54"/>
+      <c r="AH13" s="54"/>
+      <c r="AI13" s="54"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="55"/>
+      <c r="B14" s="55">
+        <v>9009.0</v>
+      </c>
+      <c r="C14" s="51" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="52">
+        <v>0.2</v>
+      </c>
+      <c r="F14" s="52">
+        <v>35.0</v>
+      </c>
+      <c r="G14" s="52">
+        <v>5.0</v>
+      </c>
+      <c r="H14" s="51" t="s">
+        <v>40</v>
+      </c>
+      <c r="I14" s="56" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="K14" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="L14" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="M14" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="N14" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="O14" s="52">
+        <v>6.0</v>
+      </c>
+      <c r="P14" s="52">
+        <v>13500.0</v>
+      </c>
+      <c r="Q14" s="57"/>
+      <c r="R14" s="57"/>
+      <c r="S14" s="57"/>
+      <c r="T14" s="57"/>
+      <c r="U14" s="57"/>
+      <c r="V14" s="57"/>
+      <c r="W14" s="57"/>
+      <c r="X14" s="57"/>
+      <c r="Y14" s="57"/>
+      <c r="Z14" s="57"/>
+      <c r="AA14" s="57"/>
+      <c r="AB14" s="57"/>
+      <c r="AC14" s="57"/>
+      <c r="AD14" s="57"/>
+      <c r="AE14" s="57"/>
+      <c r="AF14" s="57"/>
+      <c r="AG14" s="57"/>
+      <c r="AH14" s="57"/>
+      <c r="AI14" s="57"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="58"/>
+      <c r="B15" s="58">
+        <v>9010.0</v>
+      </c>
+      <c r="C15" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="31">
+        <v>0.2</v>
+      </c>
+      <c r="F15" s="31">
+        <v>35.0</v>
+      </c>
+      <c r="G15" s="31">
+        <v>11.0</v>
+      </c>
+      <c r="H15" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="I15" s="31"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="31"/>
+      <c r="L15" s="31"/>
+      <c r="M15" s="31"/>
+      <c r="N15" s="59"/>
+      <c r="O15" s="59"/>
+      <c r="P15" s="60"/>
+      <c r="Q15" s="60"/>
+      <c r="R15" s="60"/>
+      <c r="S15" s="60"/>
+      <c r="T15" s="60"/>
+      <c r="U15" s="60"/>
+      <c r="V15" s="60"/>
+      <c r="W15" s="60"/>
+      <c r="X15" s="60"/>
+      <c r="Y15" s="60"/>
+      <c r="Z15" s="60"/>
+      <c r="AA15" s="60"/>
+      <c r="AB15" s="60"/>
+      <c r="AC15" s="60"/>
+      <c r="AD15" s="60"/>
+      <c r="AE15" s="60"/>
+      <c r="AF15" s="60"/>
+      <c r="AG15" s="60"/>
+      <c r="AH15" s="60"/>
+      <c r="AI15" s="60"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="61"/>
+      <c r="B16" s="58">
+        <v>9011.0</v>
+      </c>
+      <c r="C16" s="62" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="63" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="63">
+        <v>0.2</v>
+      </c>
+      <c r="F16" s="64"/>
+      <c r="G16" s="63">
+        <v>11.0</v>
+      </c>
+      <c r="H16" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="I16" s="62" t="s">
+        <v>47</v>
+      </c>
+      <c r="J16" s="65" t="s">
+        <v>30</v>
+      </c>
+      <c r="K16" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="L16" s="63">
+        <v>4.0</v>
+      </c>
+      <c r="M16" s="16">
         <v>10000.0</v>
       </c>
-      <c r="N6" s="23">
-        <v>2.544E8</v>
-      </c>
-      <c r="O6" s="21">
+      <c r="N16" s="16">
+        <v>3.576E8</v>
+      </c>
+      <c r="O16" s="65">
         <v>7.0</v>
       </c>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="24"/>
-      <c r="R6" s="24"/>
-      <c r="S6" s="24"/>
-      <c r="T6" s="24"/>
-      <c r="U6" s="24"/>
-      <c r="V6" s="24"/>
-      <c r="W6" s="24"/>
-      <c r="X6" s="24"/>
-      <c r="Y6" s="24"/>
-      <c r="Z6" s="24"/>
-      <c r="AA6" s="24"/>
-      <c r="AB6" s="24"/>
-      <c r="AC6" s="24"/>
-      <c r="AD6" s="24"/>
-      <c r="AE6" s="24"/>
-      <c r="AF6" s="24"/>
-      <c r="AG6" s="24"/>
-      <c r="AH6" s="24"/>
-      <c r="AI6" s="24"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="25" t="s">
+      <c r="P16" s="66"/>
+      <c r="Q16" s="66"/>
+      <c r="R16" s="66"/>
+      <c r="S16" s="66"/>
+      <c r="T16" s="66"/>
+      <c r="U16" s="66"/>
+      <c r="V16" s="66"/>
+      <c r="W16" s="66"/>
+      <c r="X16" s="66"/>
+      <c r="Y16" s="66"/>
+      <c r="Z16" s="66"/>
+      <c r="AA16" s="66"/>
+      <c r="AB16" s="66"/>
+      <c r="AC16" s="66"/>
+      <c r="AD16" s="66"/>
+      <c r="AE16" s="66"/>
+      <c r="AF16" s="66"/>
+      <c r="AG16" s="66"/>
+      <c r="AH16" s="66"/>
+      <c r="AI16" s="66"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="67"/>
+      <c r="B17" s="68">
+        <v>9012.0</v>
+      </c>
+      <c r="C17" s="69" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="70" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="70">
+        <v>0.2</v>
+      </c>
+      <c r="F17" s="70">
+        <v>35.0</v>
+      </c>
+      <c r="G17" s="70">
+        <v>11.0</v>
+      </c>
+      <c r="H17" s="70" t="s">
+        <v>49</v>
+      </c>
+      <c r="I17" s="69" t="s">
+        <v>50</v>
+      </c>
+      <c r="J17" s="70" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" s="70">
+        <v>5.0</v>
+      </c>
+      <c r="L17" s="71"/>
+      <c r="M17" s="71"/>
+      <c r="N17" s="71"/>
+      <c r="O17" s="70" t="s">
+        <v>51</v>
+      </c>
+      <c r="P17" s="72"/>
+      <c r="Q17" s="72"/>
+      <c r="R17" s="72"/>
+      <c r="S17" s="72"/>
+      <c r="T17" s="72"/>
+      <c r="U17" s="72"/>
+      <c r="V17" s="72"/>
+      <c r="W17" s="72"/>
+      <c r="X17" s="72"/>
+      <c r="Y17" s="72"/>
+      <c r="Z17" s="72"/>
+      <c r="AA17" s="72"/>
+      <c r="AB17" s="72"/>
+      <c r="AC17" s="72"/>
+      <c r="AD17" s="72"/>
+      <c r="AE17" s="72"/>
+      <c r="AF17" s="72"/>
+      <c r="AG17" s="72"/>
+      <c r="AH17" s="72"/>
+      <c r="AI17" s="72"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="73"/>
+      <c r="B18" s="73"/>
+      <c r="C18" s="73"/>
+      <c r="D18" s="73"/>
+      <c r="E18" s="73"/>
+      <c r="F18" s="73"/>
+      <c r="G18" s="73"/>
+      <c r="H18" s="73"/>
+      <c r="I18" s="69" t="s">
+        <v>50</v>
+      </c>
+      <c r="J18" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="25">
-        <v>9005.0</v>
-      </c>
-      <c r="C7" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="27">
-        <v>0.2</v>
-      </c>
-      <c r="F7" s="28"/>
-      <c r="G7" s="27">
-        <v>11.0</v>
-      </c>
-      <c r="H7" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="I7" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="J7" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="K7" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="L7" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="M7" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="N7" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="O7" s="27">
-        <v>8.0</v>
-      </c>
-      <c r="P7" s="27">
-        <v>13500.0</v>
-      </c>
-      <c r="Q7" s="29"/>
-      <c r="R7" s="29"/>
-      <c r="S7" s="29"/>
-      <c r="T7" s="29"/>
-      <c r="U7" s="29"/>
-      <c r="V7" s="29"/>
-      <c r="W7" s="29"/>
-      <c r="X7" s="29"/>
-      <c r="Y7" s="29"/>
-      <c r="Z7" s="29"/>
-      <c r="AA7" s="29"/>
-      <c r="AB7" s="29"/>
-      <c r="AC7" s="29"/>
-      <c r="AD7" s="29"/>
-      <c r="AE7" s="29"/>
-      <c r="AF7" s="29"/>
-      <c r="AG7" s="29"/>
-      <c r="AH7" s="29"/>
-      <c r="AI7" s="29"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="30"/>
-      <c r="B8" s="30">
-        <v>9006.0</v>
-      </c>
-      <c r="C8" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="32" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="32">
-        <v>0.2</v>
-      </c>
-      <c r="F8" s="32">
-        <v>35.0</v>
-      </c>
-      <c r="G8" s="32">
-        <v>5.0</v>
-      </c>
-      <c r="H8" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="I8" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="J8" s="32" t="s">
-        <v>23</v>
-      </c>
-      <c r="K8" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="L8" s="32">
-        <v>4.0</v>
-      </c>
-      <c r="M8" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="N8" s="32">
-        <v>3.408E8</v>
-      </c>
-      <c r="O8" s="32">
-        <v>6.0</v>
-      </c>
-      <c r="P8" s="34"/>
-      <c r="Q8" s="34"/>
-      <c r="R8" s="34"/>
-      <c r="S8" s="34"/>
-      <c r="T8" s="34"/>
-      <c r="U8" s="34"/>
-      <c r="V8" s="34"/>
-      <c r="W8" s="34"/>
-      <c r="X8" s="34"/>
-      <c r="Y8" s="34"/>
-      <c r="Z8" s="34"/>
-      <c r="AA8" s="34"/>
-      <c r="AB8" s="34"/>
-      <c r="AC8" s="34"/>
-      <c r="AD8" s="34"/>
-      <c r="AE8" s="34"/>
-      <c r="AF8" s="34"/>
-      <c r="AG8" s="34"/>
-      <c r="AH8" s="34"/>
-      <c r="AI8" s="34"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="35"/>
-      <c r="B9" s="35">
-        <v>9007.0</v>
-      </c>
-      <c r="C9" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="32" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="32">
-        <v>0.2</v>
-      </c>
-      <c r="F9" s="32">
-        <v>35.0</v>
-      </c>
-      <c r="G9" s="36">
-        <v>5.0</v>
-      </c>
-      <c r="H9" s="37" t="s">
-        <v>38</v>
-      </c>
-      <c r="I9" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="J9" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="K9" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="L9" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="M9" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="N9" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="O9" s="38"/>
-      <c r="P9" s="39"/>
-      <c r="Q9" s="39"/>
-      <c r="R9" s="39"/>
-      <c r="S9" s="39"/>
-      <c r="T9" s="39"/>
-      <c r="U9" s="39"/>
-      <c r="V9" s="39"/>
-      <c r="W9" s="39"/>
-      <c r="X9" s="39"/>
-      <c r="Y9" s="39"/>
-      <c r="Z9" s="39"/>
-      <c r="AA9" s="39"/>
-      <c r="AB9" s="39"/>
-      <c r="AC9" s="39"/>
-      <c r="AD9" s="39"/>
-      <c r="AE9" s="39"/>
-      <c r="AF9" s="39"/>
-      <c r="AG9" s="39"/>
-      <c r="AH9" s="39"/>
-      <c r="AI9" s="39"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="40"/>
-      <c r="B10" s="40">
-        <v>9008.0</v>
-      </c>
-      <c r="C10" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="42">
-        <v>0.2</v>
-      </c>
-      <c r="F10" s="42">
-        <v>35.0</v>
-      </c>
-      <c r="G10" s="42">
-        <v>5.0</v>
-      </c>
-      <c r="H10" s="41" t="s">
-        <v>38</v>
-      </c>
-      <c r="I10" s="43" t="s">
-        <v>40</v>
-      </c>
-      <c r="J10" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="K10" s="42" t="s">
-        <v>17</v>
-      </c>
-      <c r="L10" s="42">
-        <v>4.0</v>
-      </c>
-      <c r="M10" s="42">
-        <v>11000.0</v>
-      </c>
-      <c r="N10" s="42">
-        <v>3.392E8</v>
-      </c>
-      <c r="O10" s="42">
-        <v>7.0</v>
-      </c>
-      <c r="P10" s="44"/>
-      <c r="Q10" s="44"/>
-      <c r="R10" s="44"/>
-      <c r="S10" s="44"/>
-      <c r="T10" s="44"/>
-      <c r="U10" s="44"/>
-      <c r="V10" s="44"/>
-      <c r="W10" s="44"/>
-      <c r="X10" s="44"/>
-      <c r="Y10" s="44"/>
-      <c r="Z10" s="44"/>
-      <c r="AA10" s="44"/>
-      <c r="AB10" s="44"/>
-      <c r="AC10" s="44"/>
-      <c r="AD10" s="44"/>
-      <c r="AE10" s="44"/>
-      <c r="AF10" s="44"/>
-      <c r="AG10" s="44"/>
-      <c r="AH10" s="44"/>
-      <c r="AI10" s="44"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="45"/>
-      <c r="B11" s="45">
-        <v>9009.0</v>
-      </c>
-      <c r="C11" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="42">
-        <v>0.2</v>
-      </c>
-      <c r="F11" s="42">
-        <v>35.0</v>
-      </c>
-      <c r="G11" s="42">
-        <v>5.0</v>
-      </c>
-      <c r="H11" s="41" t="s">
-        <v>38</v>
-      </c>
-      <c r="I11" s="43" t="s">
-        <v>40</v>
-      </c>
-      <c r="J11" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="K11" s="42" t="s">
-        <v>29</v>
-      </c>
-      <c r="L11" s="42" t="s">
-        <v>33</v>
-      </c>
-      <c r="M11" s="42" t="s">
-        <v>33</v>
-      </c>
-      <c r="N11" s="42" t="s">
-        <v>33</v>
-      </c>
-      <c r="O11" s="42">
-        <v>6.0</v>
-      </c>
-      <c r="P11" s="42">
-        <v>13500.0</v>
-      </c>
-      <c r="Q11" s="46"/>
-      <c r="R11" s="46"/>
-      <c r="S11" s="46"/>
-      <c r="T11" s="46"/>
-      <c r="U11" s="46"/>
-      <c r="V11" s="46"/>
-      <c r="W11" s="46"/>
-      <c r="X11" s="46"/>
-      <c r="Y11" s="46"/>
-      <c r="Z11" s="46"/>
-      <c r="AA11" s="46"/>
-      <c r="AB11" s="46"/>
-      <c r="AC11" s="46"/>
-      <c r="AD11" s="46"/>
-      <c r="AE11" s="46"/>
-      <c r="AF11" s="46"/>
-      <c r="AG11" s="46"/>
-      <c r="AH11" s="46"/>
-      <c r="AI11" s="46"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="47"/>
-      <c r="B12" s="47">
-        <v>9010.0</v>
-      </c>
-      <c r="C12" s="48" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="49" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="49">
-        <v>0.2</v>
-      </c>
-      <c r="F12" s="49">
-        <v>35.0</v>
-      </c>
-      <c r="G12" s="49">
-        <v>11.0</v>
-      </c>
-      <c r="H12" s="49"/>
-      <c r="I12" s="49"/>
-      <c r="J12" s="49"/>
-      <c r="K12" s="49"/>
-      <c r="L12" s="49"/>
-      <c r="M12" s="50" t="s">
-        <v>43</v>
-      </c>
-      <c r="N12" s="51"/>
-      <c r="O12" s="51"/>
-      <c r="P12" s="52"/>
-      <c r="Q12" s="52"/>
-      <c r="R12" s="52"/>
-      <c r="S12" s="52"/>
-      <c r="T12" s="52"/>
-      <c r="U12" s="52"/>
-      <c r="V12" s="52"/>
-      <c r="W12" s="52"/>
-      <c r="X12" s="52"/>
-      <c r="Y12" s="52"/>
-      <c r="Z12" s="52"/>
-      <c r="AA12" s="52"/>
-      <c r="AB12" s="52"/>
-      <c r="AC12" s="52"/>
-      <c r="AD12" s="52"/>
-      <c r="AE12" s="52"/>
-      <c r="AF12" s="52"/>
-      <c r="AG12" s="52"/>
-      <c r="AH12" s="52"/>
-      <c r="AI12" s="52"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="53"/>
-      <c r="B13" s="47">
-        <v>9011.0</v>
-      </c>
-      <c r="C13" s="54" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" s="55" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="55">
-        <v>0.2</v>
-      </c>
-      <c r="F13" s="56"/>
-      <c r="G13" s="55">
-        <v>11.0</v>
-      </c>
-      <c r="H13" s="55" t="s">
-        <v>27</v>
-      </c>
-      <c r="I13" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="J13" s="55" t="s">
-        <v>23</v>
-      </c>
-      <c r="K13" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="L13" s="55">
-        <v>4.0</v>
-      </c>
-      <c r="M13" s="57" t="s">
-        <v>46</v>
-      </c>
-      <c r="N13" s="56"/>
-      <c r="O13" s="56"/>
-      <c r="P13" s="58"/>
-      <c r="Q13" s="58"/>
-      <c r="R13" s="58"/>
-      <c r="S13" s="58"/>
-      <c r="T13" s="58"/>
-      <c r="U13" s="58"/>
-      <c r="V13" s="58"/>
-      <c r="W13" s="58"/>
-      <c r="X13" s="58"/>
-      <c r="Y13" s="58"/>
-      <c r="Z13" s="58"/>
-      <c r="AA13" s="58"/>
-      <c r="AB13" s="58"/>
-      <c r="AC13" s="58"/>
-      <c r="AD13" s="58"/>
-      <c r="AE13" s="58"/>
-      <c r="AF13" s="58"/>
-      <c r="AG13" s="58"/>
-      <c r="AH13" s="58"/>
-      <c r="AI13" s="58"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="59"/>
-      <c r="B14" s="59">
-        <v>9012.0</v>
-      </c>
-      <c r="C14" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14" s="60"/>
-      <c r="E14" s="61"/>
-      <c r="F14" s="62"/>
-      <c r="G14" s="62"/>
-      <c r="H14" s="62"/>
-      <c r="I14" s="62"/>
-      <c r="J14" s="62"/>
-      <c r="K14" s="62"/>
-      <c r="L14" s="62"/>
-      <c r="M14" s="62"/>
-      <c r="N14" s="62"/>
-      <c r="O14" s="13"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="63" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="63">
-        <v>9013.0</v>
-      </c>
-      <c r="C15" s="64" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" s="65" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="65">
-        <v>0.2</v>
-      </c>
-      <c r="F15" s="66"/>
-      <c r="G15" s="65">
-        <v>11.0</v>
-      </c>
-      <c r="H15" s="65" t="s">
-        <v>27</v>
-      </c>
-      <c r="I15" s="64" t="s">
-        <v>22</v>
-      </c>
-      <c r="J15" s="65" t="s">
-        <v>31</v>
-      </c>
-      <c r="K15" s="65" t="s">
-        <v>29</v>
-      </c>
-      <c r="L15" s="65" t="s">
-        <v>33</v>
-      </c>
-      <c r="M15" s="65" t="s">
-        <v>33</v>
-      </c>
-      <c r="N15" s="65" t="s">
-        <v>33</v>
-      </c>
-      <c r="O15" s="67">
-        <v>7.0</v>
-      </c>
-      <c r="P15" s="64" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q15" s="68"/>
-      <c r="R15" s="68"/>
-      <c r="S15" s="68"/>
-      <c r="T15" s="68"/>
-      <c r="U15" s="68"/>
-      <c r="V15" s="68"/>
-      <c r="W15" s="68"/>
-      <c r="X15" s="68"/>
-      <c r="Y15" s="68"/>
-      <c r="Z15" s="68"/>
-      <c r="AA15" s="68"/>
-      <c r="AB15" s="68"/>
-      <c r="AC15" s="68"/>
-      <c r="AD15" s="68"/>
-      <c r="AE15" s="68"/>
-      <c r="AF15" s="68"/>
-      <c r="AG15" s="68"/>
-      <c r="AH15" s="68"/>
-      <c r="AI15" s="68"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="25"/>
-      <c r="B16" s="69">
-        <v>9014.0</v>
-      </c>
-      <c r="C16" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="E16" s="27">
-        <v>0.2</v>
-      </c>
-      <c r="F16" s="28"/>
-      <c r="G16" s="27">
-        <v>11.0</v>
-      </c>
-      <c r="H16" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="I16" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="J16" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="K16" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="L16" s="27">
-        <v>4.0</v>
-      </c>
-      <c r="M16" s="70" t="s">
-        <v>50</v>
-      </c>
-      <c r="N16" s="28"/>
-      <c r="O16" s="28"/>
-      <c r="P16" s="29"/>
-      <c r="Q16" s="29"/>
-      <c r="R16" s="29"/>
-      <c r="S16" s="29"/>
-      <c r="T16" s="29"/>
-      <c r="U16" s="29"/>
-      <c r="V16" s="29"/>
-      <c r="W16" s="29"/>
-      <c r="X16" s="29"/>
-      <c r="Y16" s="29"/>
-      <c r="Z16" s="29"/>
-      <c r="AA16" s="29"/>
-      <c r="AB16" s="29"/>
-      <c r="AC16" s="29"/>
-      <c r="AD16" s="29"/>
-      <c r="AE16" s="29"/>
-      <c r="AF16" s="29"/>
-      <c r="AG16" s="29"/>
-      <c r="AH16" s="29"/>
-      <c r="AI16" s="29"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
-      <c r="O17" s="13"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="11" t="s">
+      <c r="K18" s="73"/>
+      <c r="L18" s="73"/>
+      <c r="M18" s="73"/>
+      <c r="N18" s="73"/>
+      <c r="O18" s="73"/>
+      <c r="P18" s="73"/>
+      <c r="Q18" s="73"/>
+      <c r="R18" s="73"/>
+      <c r="S18" s="73"/>
+      <c r="T18" s="73"/>
+      <c r="U18" s="73"/>
+      <c r="V18" s="73"/>
+      <c r="W18" s="73"/>
+      <c r="X18" s="73"/>
+      <c r="Y18" s="73"/>
+      <c r="Z18" s="73"/>
+      <c r="AA18" s="73"/>
+      <c r="AB18" s="73"/>
+      <c r="AC18" s="73"/>
+      <c r="AD18" s="73"/>
+      <c r="AE18" s="73"/>
+      <c r="AF18" s="73"/>
+      <c r="AG18" s="73"/>
+      <c r="AH18" s="73"/>
+      <c r="AI18" s="73"/>
+    </row>
+    <row r="19">
+      <c r="H19" s="74" t="s">
         <v>52</v>
       </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
-      <c r="N18" s="13"/>
-      <c r="O18" s="13"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="71"/>
-      <c r="G19" s="71"/>
-      <c r="H19" s="72" t="s">
-        <v>53</v>
-      </c>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
-      <c r="O19" s="13"/>
     </row>
     <row r="20">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
+      <c r="C20" s="11" t="s">
+        <v>53</v>
+      </c>
       <c r="D20" s="13"/>
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="G20" s="12"/>
       <c r="H20" s="13"/>
       <c r="I20" s="13"/>
       <c r="J20" s="13"/>
@@ -1834,6 +1941,9 @@
     <row r="21">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
+      <c r="C21" s="11" t="s">
+        <v>54</v>
+      </c>
       <c r="D21" s="13"/>
       <c r="E21" s="13"/>
       <c r="F21" s="13"/>
@@ -1852,11 +1962,15 @@
       <c r="B22" s="1"/>
       <c r="D22" s="13"/>
       <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
+      <c r="F22" s="75"/>
+      <c r="G22" s="75"/>
+      <c r="H22" s="76" t="s">
+        <v>55</v>
+      </c>
       <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
+      <c r="J22" s="12" t="s">
+        <v>56</v>
+      </c>
       <c r="K22" s="13"/>
       <c r="L22" s="13"/>
       <c r="M22" s="13"/>
@@ -17527,6 +17641,54 @@
       <c r="N1001" s="13"/>
       <c r="O1001" s="13"/>
     </row>
+    <row r="1002">
+      <c r="A1002" s="1"/>
+      <c r="B1002" s="1"/>
+      <c r="D1002" s="13"/>
+      <c r="E1002" s="13"/>
+      <c r="F1002" s="13"/>
+      <c r="G1002" s="13"/>
+      <c r="H1002" s="13"/>
+      <c r="I1002" s="13"/>
+      <c r="J1002" s="13"/>
+      <c r="K1002" s="13"/>
+      <c r="L1002" s="13"/>
+      <c r="M1002" s="13"/>
+      <c r="N1002" s="13"/>
+      <c r="O1002" s="13"/>
+    </row>
+    <row r="1003">
+      <c r="A1003" s="1"/>
+      <c r="B1003" s="1"/>
+      <c r="D1003" s="13"/>
+      <c r="E1003" s="13"/>
+      <c r="F1003" s="13"/>
+      <c r="G1003" s="13"/>
+      <c r="H1003" s="13"/>
+      <c r="I1003" s="13"/>
+      <c r="J1003" s="13"/>
+      <c r="K1003" s="13"/>
+      <c r="L1003" s="13"/>
+      <c r="M1003" s="13"/>
+      <c r="N1003" s="13"/>
+      <c r="O1003" s="13"/>
+    </row>
+    <row r="1004">
+      <c r="A1004" s="1"/>
+      <c r="B1004" s="1"/>
+      <c r="D1004" s="13"/>
+      <c r="E1004" s="13"/>
+      <c r="F1004" s="13"/>
+      <c r="G1004" s="13"/>
+      <c r="H1004" s="13"/>
+      <c r="I1004" s="13"/>
+      <c r="J1004" s="13"/>
+      <c r="K1004" s="13"/>
+      <c r="L1004" s="13"/>
+      <c r="M1004" s="13"/>
+      <c r="N1004" s="13"/>
+      <c r="O1004" s="13"/>
+    </row>
   </sheetData>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>

</xml_diff>

<commit_message>
actualizado 9 oct 19.20 hs
</commit_message>
<xml_diff>
--- a/competencia 01 bitácora.xlsx
+++ b/competencia 01 bitácora.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="56">
   <si>
     <t>dataset</t>
   </si>
@@ -133,9 +133,6 @@
     <t>10500-12000, 13500</t>
   </si>
   <si>
-    <t>*</t>
-  </si>
-  <si>
     <t>fe lags deltas 1,2,3 (9005)</t>
   </si>
   <si>
@@ -196,16 +193,22 @@
     <t xml:space="preserve">fe lags deltas 1,2,3 y ag </t>
   </si>
   <si>
+    <t>*</t>
+  </si>
+  <si>
     <t>fe123_rank</t>
   </si>
   <si>
-    <t>auc = 0.9447</t>
+    <t>stop#36. auc = 0.9447</t>
   </si>
   <si>
     <t>fe123_rank_agui</t>
   </si>
   <si>
-    <t>rserver</t>
+    <t>reoptimizar</t>
+  </si>
+  <si>
+    <t>escalar min data leaf</t>
   </si>
   <si>
     <t>9002 new 0.9448/50</t>
@@ -216,18 +219,12 @@
   <si>
     <t>*a mismo modelo, incluir aguinaldo en 06 rindió peor en kaggle (7 versus 6)</t>
   </si>
-  <si>
-    <t>terminar de optimizar 9002 con min data 3</t>
-  </si>
-  <si>
-    <t>colab</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -352,13 +349,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11.0"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="9.0"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -421,7 +411,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="75">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -496,9 +486,6 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
@@ -596,17 +583,11 @@
     <xf borderId="0" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf borderId="0" fillId="4" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="8" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="8" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="8" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -615,12 +596,15 @@
     <xf borderId="0" fillId="8" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="8" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
+    <xf borderId="0" fillId="8" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="8" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="8" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="8" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1191,14 +1175,12 @@
       <c r="AI6" s="25"/>
     </row>
     <row r="7">
-      <c r="A7" s="21" t="s">
-        <v>27</v>
-      </c>
+      <c r="A7" s="21"/>
       <c r="B7" s="21">
         <v>9013.0</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" s="18" t="s">
         <v>23</v>
@@ -1206,36 +1188,38 @@
       <c r="E7" s="18">
         <v>0.2</v>
       </c>
-      <c r="F7" s="26"/>
+      <c r="F7" s="18">
+        <v>30.0</v>
+      </c>
       <c r="G7" s="18">
         <v>11.0</v>
       </c>
       <c r="H7" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I7" s="22" t="s">
         <v>22</v>
       </c>
       <c r="J7" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="K7" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="K7" s="18" t="s">
+      <c r="L7" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="L7" s="18" t="s">
-        <v>32</v>
-      </c>
       <c r="M7" s="18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N7" s="18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O7" s="23">
         <v>7.0</v>
       </c>
       <c r="P7" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Q7" s="25"/>
       <c r="R7" s="25"/>
@@ -1258,530 +1242,538 @@
       <c r="AI7" s="25"/>
     </row>
     <row r="8">
-      <c r="A8" s="27"/>
-      <c r="B8" s="27">
+      <c r="A8" s="26"/>
+      <c r="B8" s="26">
         <v>9004.0</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="29">
+      <c r="E8" s="28">
         <v>0.2</v>
       </c>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29">
+      <c r="F8" s="28">
+        <v>30.0</v>
+      </c>
+      <c r="G8" s="28">
         <v>11.0</v>
       </c>
-      <c r="H8" s="29" t="s">
+      <c r="H8" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="J8" s="30">
+        <v>2.0</v>
+      </c>
+      <c r="K8" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="L8" s="30">
+        <v>3.0</v>
+      </c>
+      <c r="M8" s="30">
+        <v>10000.0</v>
+      </c>
+      <c r="N8" s="30">
+        <v>2.544E8</v>
+      </c>
+      <c r="O8" s="28">
+        <v>7.0</v>
+      </c>
+      <c r="P8" s="31"/>
+      <c r="Q8" s="31"/>
+      <c r="R8" s="31"/>
+      <c r="S8" s="31"/>
+      <c r="T8" s="31"/>
+      <c r="U8" s="31"/>
+      <c r="V8" s="31"/>
+      <c r="W8" s="31"/>
+      <c r="X8" s="31"/>
+      <c r="Y8" s="31"/>
+      <c r="Z8" s="31"/>
+      <c r="AA8" s="31"/>
+      <c r="AB8" s="31"/>
+      <c r="AC8" s="31"/>
+      <c r="AD8" s="31"/>
+      <c r="AE8" s="31"/>
+      <c r="AF8" s="31"/>
+      <c r="AG8" s="31"/>
+      <c r="AH8" s="31"/>
+      <c r="AI8" s="31"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="32"/>
+      <c r="B9" s="33">
+        <v>9014.0</v>
+      </c>
+      <c r="C9" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="35">
+        <v>0.2</v>
+      </c>
+      <c r="F9" s="35">
+        <v>30.0</v>
+      </c>
+      <c r="G9" s="35">
+        <v>11.0</v>
+      </c>
+      <c r="H9" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="K9" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="L9" s="35">
+        <v>4.0</v>
+      </c>
+      <c r="M9" s="35">
+        <v>9000.0</v>
+      </c>
+      <c r="N9" s="35">
+        <v>3.544E8</v>
+      </c>
+      <c r="O9" s="36"/>
+      <c r="P9" s="37"/>
+      <c r="Q9" s="37"/>
+      <c r="R9" s="37"/>
+      <c r="S9" s="37"/>
+      <c r="T9" s="37"/>
+      <c r="U9" s="37"/>
+      <c r="V9" s="37"/>
+      <c r="W9" s="37"/>
+      <c r="X9" s="37"/>
+      <c r="Y9" s="37"/>
+      <c r="Z9" s="37"/>
+      <c r="AA9" s="37"/>
+      <c r="AB9" s="37"/>
+      <c r="AC9" s="37"/>
+      <c r="AD9" s="37"/>
+      <c r="AE9" s="37"/>
+      <c r="AF9" s="37"/>
+      <c r="AG9" s="37"/>
+      <c r="AH9" s="37"/>
+      <c r="AI9" s="37"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="32"/>
+      <c r="B10" s="32">
+        <v>9005.0</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="35">
+        <v>0.2</v>
+      </c>
+      <c r="F10" s="35">
+        <v>30.0</v>
+      </c>
+      <c r="G10" s="35">
+        <v>11.0</v>
+      </c>
+      <c r="H10" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="J10" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="I8" s="30" t="s">
+      <c r="K10" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="31">
-        <v>2.0</v>
-      </c>
-      <c r="K8" s="31" t="s">
+      <c r="L10" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="L8" s="31">
-        <v>3.0</v>
-      </c>
-      <c r="M8" s="31">
-        <v>10000.0</v>
-      </c>
-      <c r="N8" s="31">
-        <v>2.544E8</v>
-      </c>
-      <c r="O8" s="29">
+      <c r="M10" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="N10" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="O10" s="35">
+        <v>8.0</v>
+      </c>
+      <c r="P10" s="35">
+        <v>13500.0</v>
+      </c>
+      <c r="Q10" s="37"/>
+      <c r="R10" s="37"/>
+      <c r="S10" s="37"/>
+      <c r="T10" s="37"/>
+      <c r="U10" s="37"/>
+      <c r="V10" s="37"/>
+      <c r="W10" s="37"/>
+      <c r="X10" s="37"/>
+      <c r="Y10" s="37"/>
+      <c r="Z10" s="37"/>
+      <c r="AA10" s="37"/>
+      <c r="AB10" s="37"/>
+      <c r="AC10" s="37"/>
+      <c r="AD10" s="37"/>
+      <c r="AE10" s="37"/>
+      <c r="AF10" s="37"/>
+      <c r="AG10" s="37"/>
+      <c r="AH10" s="37"/>
+      <c r="AI10" s="37"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="38"/>
+      <c r="B11" s="38">
+        <v>9006.0</v>
+      </c>
+      <c r="C11" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="40">
+        <v>0.2</v>
+      </c>
+      <c r="F11" s="40">
+        <v>35.0</v>
+      </c>
+      <c r="G11" s="40">
+        <v>5.0</v>
+      </c>
+      <c r="H11" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="I11" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="J11" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="K11" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="L11" s="40">
+        <v>4.0</v>
+      </c>
+      <c r="M11" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="N11" s="40">
+        <v>3.408E8</v>
+      </c>
+      <c r="O11" s="40">
+        <v>6.0</v>
+      </c>
+      <c r="P11" s="43"/>
+      <c r="Q11" s="43"/>
+      <c r="R11" s="43"/>
+      <c r="S11" s="43"/>
+      <c r="T11" s="43"/>
+      <c r="U11" s="43"/>
+      <c r="V11" s="43"/>
+      <c r="W11" s="43"/>
+      <c r="X11" s="43"/>
+      <c r="Y11" s="43"/>
+      <c r="Z11" s="43"/>
+      <c r="AA11" s="43"/>
+      <c r="AB11" s="43"/>
+      <c r="AC11" s="43"/>
+      <c r="AD11" s="43"/>
+      <c r="AE11" s="43"/>
+      <c r="AF11" s="43"/>
+      <c r="AG11" s="43"/>
+      <c r="AH11" s="43"/>
+      <c r="AI11" s="43"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="44"/>
+      <c r="B12" s="44">
+        <v>9007.0</v>
+      </c>
+      <c r="C12" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="46">
+        <v>0.2</v>
+      </c>
+      <c r="F12" s="46">
+        <v>35.0</v>
+      </c>
+      <c r="G12" s="46">
+        <v>5.0</v>
+      </c>
+      <c r="H12" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="I12" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="J12" s="46" t="s">
+        <v>29</v>
+      </c>
+      <c r="K12" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="L12" s="46"/>
+      <c r="M12" s="46"/>
+      <c r="N12" s="46"/>
+      <c r="O12" s="47"/>
+      <c r="P12" s="48"/>
+      <c r="Q12" s="48"/>
+      <c r="R12" s="48"/>
+      <c r="S12" s="48"/>
+      <c r="T12" s="48"/>
+      <c r="U12" s="48"/>
+      <c r="V12" s="48"/>
+      <c r="W12" s="48"/>
+      <c r="X12" s="48"/>
+      <c r="Y12" s="48"/>
+      <c r="Z12" s="48"/>
+      <c r="AA12" s="48"/>
+      <c r="AB12" s="48"/>
+      <c r="AC12" s="48"/>
+      <c r="AD12" s="48"/>
+      <c r="AE12" s="48"/>
+      <c r="AF12" s="48"/>
+      <c r="AG12" s="48"/>
+      <c r="AH12" s="48"/>
+      <c r="AI12" s="48"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="49"/>
+      <c r="B13" s="49">
+        <v>9008.0</v>
+      </c>
+      <c r="C13" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="51">
+        <v>0.2</v>
+      </c>
+      <c r="F13" s="51">
+        <v>35.0</v>
+      </c>
+      <c r="G13" s="51">
+        <v>5.0</v>
+      </c>
+      <c r="H13" s="50" t="s">
+        <v>39</v>
+      </c>
+      <c r="I13" s="52" t="s">
+        <v>41</v>
+      </c>
+      <c r="J13" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="K13" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="L13" s="51">
+        <v>4.0</v>
+      </c>
+      <c r="M13" s="51">
+        <v>11000.0</v>
+      </c>
+      <c r="N13" s="51">
+        <v>3.392E8</v>
+      </c>
+      <c r="O13" s="51">
         <v>7.0</v>
       </c>
-      <c r="P8" s="32"/>
-      <c r="Q8" s="32"/>
-      <c r="R8" s="32"/>
-      <c r="S8" s="32"/>
-      <c r="T8" s="32"/>
-      <c r="U8" s="32"/>
-      <c r="V8" s="32"/>
-      <c r="W8" s="32"/>
-      <c r="X8" s="32"/>
-      <c r="Y8" s="32"/>
-      <c r="Z8" s="32"/>
-      <c r="AA8" s="32"/>
-      <c r="AB8" s="32"/>
-      <c r="AC8" s="32"/>
-      <c r="AD8" s="32"/>
-      <c r="AE8" s="32"/>
-      <c r="AF8" s="32"/>
-      <c r="AG8" s="32"/>
-      <c r="AH8" s="32"/>
-      <c r="AI8" s="32"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="33"/>
-      <c r="B9" s="34">
-        <v>9014.0</v>
-      </c>
-      <c r="C9" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="36" t="s">
+      <c r="P13" s="53"/>
+      <c r="Q13" s="53"/>
+      <c r="R13" s="53"/>
+      <c r="S13" s="53"/>
+      <c r="T13" s="53"/>
+      <c r="U13" s="53"/>
+      <c r="V13" s="53"/>
+      <c r="W13" s="53"/>
+      <c r="X13" s="53"/>
+      <c r="Y13" s="53"/>
+      <c r="Z13" s="53"/>
+      <c r="AA13" s="53"/>
+      <c r="AB13" s="53"/>
+      <c r="AC13" s="53"/>
+      <c r="AD13" s="53"/>
+      <c r="AE13" s="53"/>
+      <c r="AF13" s="53"/>
+      <c r="AG13" s="53"/>
+      <c r="AH13" s="53"/>
+      <c r="AI13" s="53"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="54"/>
+      <c r="B14" s="54">
+        <v>9009.0</v>
+      </c>
+      <c r="C14" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="36">
+      <c r="E14" s="51">
         <v>0.2</v>
       </c>
-      <c r="F9" s="37"/>
-      <c r="G9" s="36">
+      <c r="F14" s="51">
+        <v>35.0</v>
+      </c>
+      <c r="G14" s="51">
+        <v>5.0</v>
+      </c>
+      <c r="H14" s="50" t="s">
+        <v>39</v>
+      </c>
+      <c r="I14" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="J14" s="51" t="s">
+        <v>29</v>
+      </c>
+      <c r="K14" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="L14" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="M14" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="N14" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="O14" s="51">
+        <v>6.0</v>
+      </c>
+      <c r="P14" s="51">
+        <v>13500.0</v>
+      </c>
+      <c r="Q14" s="56"/>
+      <c r="R14" s="56"/>
+      <c r="S14" s="56"/>
+      <c r="T14" s="56"/>
+      <c r="U14" s="56"/>
+      <c r="V14" s="56"/>
+      <c r="W14" s="56"/>
+      <c r="X14" s="56"/>
+      <c r="Y14" s="56"/>
+      <c r="Z14" s="56"/>
+      <c r="AA14" s="56"/>
+      <c r="AB14" s="56"/>
+      <c r="AC14" s="56"/>
+      <c r="AD14" s="56"/>
+      <c r="AE14" s="56"/>
+      <c r="AF14" s="56"/>
+      <c r="AG14" s="56"/>
+      <c r="AH14" s="56"/>
+      <c r="AI14" s="56"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="57"/>
+      <c r="B15" s="57">
+        <v>9010.0</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="F15" s="30">
+        <v>35.0</v>
+      </c>
+      <c r="G15" s="30">
         <v>11.0</v>
       </c>
-      <c r="H9" s="36" t="s">
+      <c r="H15" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="30"/>
+      <c r="N15" s="58"/>
+      <c r="O15" s="58"/>
+      <c r="P15" s="59"/>
+      <c r="Q15" s="59"/>
+      <c r="R15" s="59"/>
+      <c r="S15" s="59"/>
+      <c r="T15" s="59"/>
+      <c r="U15" s="59"/>
+      <c r="V15" s="59"/>
+      <c r="W15" s="59"/>
+      <c r="X15" s="59"/>
+      <c r="Y15" s="59"/>
+      <c r="Z15" s="59"/>
+      <c r="AA15" s="59"/>
+      <c r="AB15" s="59"/>
+      <c r="AC15" s="59"/>
+      <c r="AD15" s="59"/>
+      <c r="AE15" s="59"/>
+      <c r="AF15" s="59"/>
+      <c r="AG15" s="59"/>
+      <c r="AH15" s="59"/>
+      <c r="AI15" s="59"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="60"/>
+      <c r="B16" s="57">
+        <v>9011.0</v>
+      </c>
+      <c r="C16" s="61" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="62" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="62">
+        <v>0.2</v>
+      </c>
+      <c r="F16" s="63">
+        <v>30.0</v>
+      </c>
+      <c r="G16" s="62">
+        <v>11.0</v>
+      </c>
+      <c r="H16" s="63" t="s">
+        <v>28</v>
+      </c>
+      <c r="I16" s="61" t="s">
+        <v>46</v>
+      </c>
+      <c r="J16" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="I9" s="35" t="s">
-        <v>34</v>
-      </c>
-      <c r="J9" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="K9" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="L9" s="36">
-        <v>4.0</v>
-      </c>
-      <c r="M9" s="36">
-        <v>9000.0</v>
-      </c>
-      <c r="N9" s="36">
-        <v>3.544E8</v>
-      </c>
-      <c r="O9" s="37"/>
-      <c r="P9" s="38"/>
-      <c r="Q9" s="38"/>
-      <c r="R9" s="38"/>
-      <c r="S9" s="38"/>
-      <c r="T9" s="38"/>
-      <c r="U9" s="38"/>
-      <c r="V9" s="38"/>
-      <c r="W9" s="38"/>
-      <c r="X9" s="38"/>
-      <c r="Y9" s="38"/>
-      <c r="Z9" s="38"/>
-      <c r="AA9" s="38"/>
-      <c r="AB9" s="38"/>
-      <c r="AC9" s="38"/>
-      <c r="AD9" s="38"/>
-      <c r="AE9" s="38"/>
-      <c r="AF9" s="38"/>
-      <c r="AG9" s="38"/>
-      <c r="AH9" s="38"/>
-      <c r="AI9" s="38"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="33"/>
-      <c r="B10" s="33">
-        <v>9005.0</v>
-      </c>
-      <c r="C10" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="36">
-        <v>0.2</v>
-      </c>
-      <c r="F10" s="37"/>
-      <c r="G10" s="36">
-        <v>11.0</v>
-      </c>
-      <c r="H10" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="I10" s="35" t="s">
-        <v>34</v>
-      </c>
-      <c r="J10" s="36" t="s">
+      <c r="K16" s="63" t="s">
         <v>30</v>
       </c>
-      <c r="K10" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="L10" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="M10" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="N10" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="O10" s="36">
-        <v>8.0</v>
-      </c>
-      <c r="P10" s="36">
-        <v>13500.0</v>
-      </c>
-      <c r="Q10" s="38"/>
-      <c r="R10" s="38"/>
-      <c r="S10" s="38"/>
-      <c r="T10" s="38"/>
-      <c r="U10" s="38"/>
-      <c r="V10" s="38"/>
-      <c r="W10" s="38"/>
-      <c r="X10" s="38"/>
-      <c r="Y10" s="38"/>
-      <c r="Z10" s="38"/>
-      <c r="AA10" s="38"/>
-      <c r="AB10" s="38"/>
-      <c r="AC10" s="38"/>
-      <c r="AD10" s="38"/>
-      <c r="AE10" s="38"/>
-      <c r="AF10" s="38"/>
-      <c r="AG10" s="38"/>
-      <c r="AH10" s="38"/>
-      <c r="AI10" s="38"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="39"/>
-      <c r="B11" s="39">
-        <v>9006.0</v>
-      </c>
-      <c r="C11" s="40" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="41" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="41">
-        <v>0.2</v>
-      </c>
-      <c r="F11" s="41">
-        <v>35.0</v>
-      </c>
-      <c r="G11" s="41">
-        <v>5.0</v>
-      </c>
-      <c r="H11" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="I11" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="J11" s="41" t="s">
-        <v>23</v>
-      </c>
-      <c r="K11" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="L11" s="41">
-        <v>4.0</v>
-      </c>
-      <c r="M11" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="N11" s="41">
-        <v>3.408E8</v>
-      </c>
-      <c r="O11" s="41">
-        <v>6.0</v>
-      </c>
-      <c r="P11" s="44"/>
-      <c r="Q11" s="44"/>
-      <c r="R11" s="44"/>
-      <c r="S11" s="44"/>
-      <c r="T11" s="44"/>
-      <c r="U11" s="44"/>
-      <c r="V11" s="44"/>
-      <c r="W11" s="44"/>
-      <c r="X11" s="44"/>
-      <c r="Y11" s="44"/>
-      <c r="Z11" s="44"/>
-      <c r="AA11" s="44"/>
-      <c r="AB11" s="44"/>
-      <c r="AC11" s="44"/>
-      <c r="AD11" s="44"/>
-      <c r="AE11" s="44"/>
-      <c r="AF11" s="44"/>
-      <c r="AG11" s="44"/>
-      <c r="AH11" s="44"/>
-      <c r="AI11" s="44"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="45"/>
-      <c r="B12" s="45">
-        <v>9007.0</v>
-      </c>
-      <c r="C12" s="46" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="47" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="47">
-        <v>0.2</v>
-      </c>
-      <c r="F12" s="47">
-        <v>35.0</v>
-      </c>
-      <c r="G12" s="47">
-        <v>5.0</v>
-      </c>
-      <c r="H12" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="I12" s="46" t="s">
-        <v>38</v>
-      </c>
-      <c r="J12" s="47" t="s">
-        <v>30</v>
-      </c>
-      <c r="K12" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="L12" s="47"/>
-      <c r="M12" s="47"/>
-      <c r="N12" s="47"/>
-      <c r="O12" s="48"/>
-      <c r="P12" s="49"/>
-      <c r="Q12" s="49"/>
-      <c r="R12" s="49"/>
-      <c r="S12" s="49"/>
-      <c r="T12" s="49"/>
-      <c r="U12" s="49"/>
-      <c r="V12" s="49"/>
-      <c r="W12" s="49"/>
-      <c r="X12" s="49"/>
-      <c r="Y12" s="49"/>
-      <c r="Z12" s="49"/>
-      <c r="AA12" s="49"/>
-      <c r="AB12" s="49"/>
-      <c r="AC12" s="49"/>
-      <c r="AD12" s="49"/>
-      <c r="AE12" s="49"/>
-      <c r="AF12" s="49"/>
-      <c r="AG12" s="49"/>
-      <c r="AH12" s="49"/>
-      <c r="AI12" s="49"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="50"/>
-      <c r="B13" s="50">
-        <v>9008.0</v>
-      </c>
-      <c r="C13" s="51" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="52">
-        <v>0.2</v>
-      </c>
-      <c r="F13" s="52">
-        <v>35.0</v>
-      </c>
-      <c r="G13" s="52">
-        <v>5.0</v>
-      </c>
-      <c r="H13" s="51" t="s">
-        <v>40</v>
-      </c>
-      <c r="I13" s="53" t="s">
-        <v>42</v>
-      </c>
-      <c r="J13" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="K13" s="52" t="s">
-        <v>17</v>
-      </c>
-      <c r="L13" s="52">
-        <v>4.0</v>
-      </c>
-      <c r="M13" s="52">
-        <v>11000.0</v>
-      </c>
-      <c r="N13" s="52">
-        <v>3.392E8</v>
-      </c>
-      <c r="O13" s="52">
-        <v>7.0</v>
-      </c>
-      <c r="P13" s="54"/>
-      <c r="Q13" s="54"/>
-      <c r="R13" s="54"/>
-      <c r="S13" s="54"/>
-      <c r="T13" s="54"/>
-      <c r="U13" s="54"/>
-      <c r="V13" s="54"/>
-      <c r="W13" s="54"/>
-      <c r="X13" s="54"/>
-      <c r="Y13" s="54"/>
-      <c r="Z13" s="54"/>
-      <c r="AA13" s="54"/>
-      <c r="AB13" s="54"/>
-      <c r="AC13" s="54"/>
-      <c r="AD13" s="54"/>
-      <c r="AE13" s="54"/>
-      <c r="AF13" s="54"/>
-      <c r="AG13" s="54"/>
-      <c r="AH13" s="54"/>
-      <c r="AI13" s="54"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="55"/>
-      <c r="B14" s="55">
-        <v>9009.0</v>
-      </c>
-      <c r="C14" s="51" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" s="52">
-        <v>0.2</v>
-      </c>
-      <c r="F14" s="52">
-        <v>35.0</v>
-      </c>
-      <c r="G14" s="52">
-        <v>5.0</v>
-      </c>
-      <c r="H14" s="51" t="s">
-        <v>40</v>
-      </c>
-      <c r="I14" s="56" t="s">
-        <v>42</v>
-      </c>
-      <c r="J14" s="52" t="s">
-        <v>30</v>
-      </c>
-      <c r="K14" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="L14" s="52" t="s">
-        <v>32</v>
-      </c>
-      <c r="M14" s="52" t="s">
-        <v>32</v>
-      </c>
-      <c r="N14" s="52" t="s">
-        <v>32</v>
-      </c>
-      <c r="O14" s="52">
-        <v>6.0</v>
-      </c>
-      <c r="P14" s="52">
-        <v>13500.0</v>
-      </c>
-      <c r="Q14" s="57"/>
-      <c r="R14" s="57"/>
-      <c r="S14" s="57"/>
-      <c r="T14" s="57"/>
-      <c r="U14" s="57"/>
-      <c r="V14" s="57"/>
-      <c r="W14" s="57"/>
-      <c r="X14" s="57"/>
-      <c r="Y14" s="57"/>
-      <c r="Z14" s="57"/>
-      <c r="AA14" s="57"/>
-      <c r="AB14" s="57"/>
-      <c r="AC14" s="57"/>
-      <c r="AD14" s="57"/>
-      <c r="AE14" s="57"/>
-      <c r="AF14" s="57"/>
-      <c r="AG14" s="57"/>
-      <c r="AH14" s="57"/>
-      <c r="AI14" s="57"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="58"/>
-      <c r="B15" s="58">
-        <v>9010.0</v>
-      </c>
-      <c r="C15" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="31">
-        <v>0.2</v>
-      </c>
-      <c r="F15" s="31">
-        <v>35.0</v>
-      </c>
-      <c r="G15" s="31">
-        <v>11.0</v>
-      </c>
-      <c r="H15" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="I15" s="31"/>
-      <c r="J15" s="31"/>
-      <c r="K15" s="31"/>
-      <c r="L15" s="31"/>
-      <c r="M15" s="31"/>
-      <c r="N15" s="59"/>
-      <c r="O15" s="59"/>
-      <c r="P15" s="60"/>
-      <c r="Q15" s="60"/>
-      <c r="R15" s="60"/>
-      <c r="S15" s="60"/>
-      <c r="T15" s="60"/>
-      <c r="U15" s="60"/>
-      <c r="V15" s="60"/>
-      <c r="W15" s="60"/>
-      <c r="X15" s="60"/>
-      <c r="Y15" s="60"/>
-      <c r="Z15" s="60"/>
-      <c r="AA15" s="60"/>
-      <c r="AB15" s="60"/>
-      <c r="AC15" s="60"/>
-      <c r="AD15" s="60"/>
-      <c r="AE15" s="60"/>
-      <c r="AF15" s="60"/>
-      <c r="AG15" s="60"/>
-      <c r="AH15" s="60"/>
-      <c r="AI15" s="60"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="61"/>
-      <c r="B16" s="58">
-        <v>9011.0</v>
-      </c>
-      <c r="C16" s="62" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16" s="63" t="s">
-        <v>23</v>
-      </c>
-      <c r="E16" s="63">
-        <v>0.2</v>
-      </c>
-      <c r="F16" s="64"/>
-      <c r="G16" s="63">
-        <v>11.0</v>
-      </c>
-      <c r="H16" s="65" t="s">
-        <v>29</v>
-      </c>
-      <c r="I16" s="62" t="s">
-        <v>47</v>
-      </c>
-      <c r="J16" s="65" t="s">
-        <v>30</v>
-      </c>
-      <c r="K16" s="65" t="s">
-        <v>31</v>
-      </c>
-      <c r="L16" s="63">
+      <c r="L16" s="62">
         <v>4.0</v>
       </c>
       <c r="M16" s="16">
@@ -1790,140 +1782,157 @@
       <c r="N16" s="16">
         <v>3.576E8</v>
       </c>
-      <c r="O16" s="65">
+      <c r="O16" s="63">
         <v>7.0</v>
       </c>
-      <c r="P16" s="66"/>
-      <c r="Q16" s="66"/>
-      <c r="R16" s="66"/>
-      <c r="S16" s="66"/>
-      <c r="T16" s="66"/>
-      <c r="U16" s="66"/>
-      <c r="V16" s="66"/>
-      <c r="W16" s="66"/>
-      <c r="X16" s="66"/>
-      <c r="Y16" s="66"/>
-      <c r="Z16" s="66"/>
-      <c r="AA16" s="66"/>
-      <c r="AB16" s="66"/>
-      <c r="AC16" s="66"/>
-      <c r="AD16" s="66"/>
-      <c r="AE16" s="66"/>
-      <c r="AF16" s="66"/>
-      <c r="AG16" s="66"/>
-      <c r="AH16" s="66"/>
-      <c r="AI16" s="66"/>
+      <c r="P16" s="64"/>
+      <c r="Q16" s="64"/>
+      <c r="R16" s="64"/>
+      <c r="S16" s="64"/>
+      <c r="T16" s="64"/>
+      <c r="U16" s="64"/>
+      <c r="V16" s="64"/>
+      <c r="W16" s="64"/>
+      <c r="X16" s="64"/>
+      <c r="Y16" s="64"/>
+      <c r="Z16" s="64"/>
+      <c r="AA16" s="64"/>
+      <c r="AB16" s="64"/>
+      <c r="AC16" s="64"/>
+      <c r="AD16" s="64"/>
+      <c r="AE16" s="64"/>
+      <c r="AF16" s="64"/>
+      <c r="AG16" s="64"/>
+      <c r="AH16" s="64"/>
+      <c r="AI16" s="64"/>
     </row>
     <row r="17">
-      <c r="A17" s="67"/>
-      <c r="B17" s="68">
+      <c r="A17" s="65" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="65">
         <v>9012.0</v>
       </c>
-      <c r="C17" s="69" t="s">
+      <c r="C17" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="70" t="s">
+      <c r="D17" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="70">
+      <c r="E17" s="67">
         <v>0.2</v>
       </c>
-      <c r="F17" s="70">
-        <v>35.0</v>
-      </c>
-      <c r="G17" s="70">
+      <c r="F17" s="67">
+        <v>50.0</v>
+      </c>
+      <c r="G17" s="67">
         <v>11.0</v>
       </c>
-      <c r="H17" s="70" t="s">
+      <c r="H17" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="I17" s="69" t="s">
+      <c r="I17" s="66" t="s">
         <v>50</v>
       </c>
-      <c r="J17" s="70" t="s">
+      <c r="J17" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="K17" s="70">
-        <v>5.0</v>
-      </c>
-      <c r="L17" s="71"/>
-      <c r="M17" s="71"/>
-      <c r="N17" s="71"/>
-      <c r="O17" s="70" t="s">
+      <c r="K17" s="67" t="s">
+        <v>17</v>
+      </c>
+      <c r="L17" s="67">
+        <v>4.0</v>
+      </c>
+      <c r="M17" s="67">
+        <v>12060.0</v>
+      </c>
+      <c r="N17" s="67">
+        <v>358800.0</v>
+      </c>
+      <c r="O17" s="67">
+        <v>8.0</v>
+      </c>
+      <c r="P17" s="66">
+        <v>12000.0</v>
+      </c>
+      <c r="Q17" s="69"/>
+      <c r="R17" s="69"/>
+      <c r="S17" s="69"/>
+      <c r="T17" s="69"/>
+      <c r="U17" s="69"/>
+      <c r="V17" s="69"/>
+      <c r="W17" s="69"/>
+      <c r="X17" s="69"/>
+      <c r="Y17" s="69"/>
+      <c r="Z17" s="69"/>
+      <c r="AA17" s="69"/>
+      <c r="AB17" s="69"/>
+      <c r="AC17" s="69"/>
+      <c r="AD17" s="69"/>
+      <c r="AE17" s="69"/>
+      <c r="AF17" s="69"/>
+      <c r="AG17" s="69"/>
+      <c r="AH17" s="69"/>
+      <c r="AI17" s="69"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="70"/>
+      <c r="B18" s="70"/>
+      <c r="C18" s="70"/>
+      <c r="D18" s="70"/>
+      <c r="E18" s="70"/>
+      <c r="F18" s="70"/>
+      <c r="G18" s="70"/>
+      <c r="H18" s="71" t="s">
         <v>51</v>
       </c>
-      <c r="P17" s="72"/>
-      <c r="Q17" s="72"/>
-      <c r="R17" s="72"/>
-      <c r="S17" s="72"/>
-      <c r="T17" s="72"/>
-      <c r="U17" s="72"/>
-      <c r="V17" s="72"/>
-      <c r="W17" s="72"/>
-      <c r="X17" s="72"/>
-      <c r="Y17" s="72"/>
-      <c r="Z17" s="72"/>
-      <c r="AA17" s="72"/>
-      <c r="AB17" s="72"/>
-      <c r="AC17" s="72"/>
-      <c r="AD17" s="72"/>
-      <c r="AE17" s="72"/>
-      <c r="AF17" s="72"/>
-      <c r="AG17" s="72"/>
-      <c r="AH17" s="72"/>
-      <c r="AI17" s="72"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="73"/>
-      <c r="B18" s="73"/>
-      <c r="C18" s="73"/>
-      <c r="D18" s="73"/>
-      <c r="E18" s="73"/>
-      <c r="F18" s="73"/>
-      <c r="G18" s="73"/>
-      <c r="H18" s="73"/>
-      <c r="I18" s="69" t="s">
+      <c r="I18" s="66" t="s">
         <v>50</v>
       </c>
-      <c r="J18" s="70" t="s">
-        <v>30</v>
-      </c>
-      <c r="K18" s="73"/>
-      <c r="L18" s="73"/>
-      <c r="M18" s="73"/>
-      <c r="N18" s="73"/>
-      <c r="O18" s="73"/>
-      <c r="P18" s="73"/>
-      <c r="Q18" s="73"/>
-      <c r="R18" s="73"/>
-      <c r="S18" s="73"/>
-      <c r="T18" s="73"/>
-      <c r="U18" s="73"/>
-      <c r="V18" s="73"/>
-      <c r="W18" s="73"/>
-      <c r="X18" s="73"/>
-      <c r="Y18" s="73"/>
-      <c r="Z18" s="73"/>
-      <c r="AA18" s="73"/>
-      <c r="AB18" s="73"/>
-      <c r="AC18" s="73"/>
-      <c r="AD18" s="73"/>
-      <c r="AE18" s="73"/>
-      <c r="AF18" s="73"/>
-      <c r="AG18" s="73"/>
-      <c r="AH18" s="73"/>
-      <c r="AI18" s="73"/>
+      <c r="J18" s="67" t="s">
+        <v>29</v>
+      </c>
+      <c r="K18" s="70"/>
+      <c r="L18" s="70"/>
+      <c r="M18" s="71" t="s">
+        <v>52</v>
+      </c>
+      <c r="N18" s="70"/>
+      <c r="O18" s="70"/>
+      <c r="P18" s="70"/>
+      <c r="Q18" s="70"/>
+      <c r="R18" s="70"/>
+      <c r="S18" s="70"/>
+      <c r="T18" s="70"/>
+      <c r="U18" s="70"/>
+      <c r="V18" s="70"/>
+      <c r="W18" s="70"/>
+      <c r="X18" s="70"/>
+      <c r="Y18" s="70"/>
+      <c r="Z18" s="70"/>
+      <c r="AA18" s="70"/>
+      <c r="AB18" s="70"/>
+      <c r="AC18" s="70"/>
+      <c r="AD18" s="70"/>
+      <c r="AE18" s="70"/>
+      <c r="AF18" s="70"/>
+      <c r="AG18" s="70"/>
+      <c r="AH18" s="70"/>
+      <c r="AI18" s="70"/>
     </row>
     <row r="19">
-      <c r="H19" s="74" t="s">
-        <v>52</v>
+      <c r="F19" s="11">
+        <v>80.0</v>
+      </c>
+      <c r="H19" s="72" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D20" s="13"/>
       <c r="E20" s="13"/>
@@ -1942,7 +1951,7 @@
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D21" s="13"/>
       <c r="E21" s="13"/>
@@ -1962,15 +1971,11 @@
       <c r="B22" s="1"/>
       <c r="D22" s="13"/>
       <c r="E22" s="13"/>
-      <c r="F22" s="75"/>
-      <c r="G22" s="75"/>
-      <c r="H22" s="76" t="s">
-        <v>55</v>
-      </c>
+      <c r="F22" s="73"/>
+      <c r="G22" s="73"/>
+      <c r="H22" s="74"/>
       <c r="I22" s="13"/>
-      <c r="J22" s="12" t="s">
-        <v>56</v>
-      </c>
+      <c r="J22" s="12"/>
       <c r="K22" s="13"/>
       <c r="L22" s="13"/>
       <c r="M22" s="13"/>

</xml_diff>